<commit_message>
- Add rownumber() in LD package to process only the first chunk of data when there are multiple embedded filed
</commit_message>
<xml_diff>
--- a/Integration Services Project/mapping/testcases-04-wo-v2.xlsx
+++ b/Integration Services Project/mapping/testcases-04-wo-v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\2023-ste-coswinmigration\02-Project Execution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EFC54-3C19-4854-8ACC-22D19450C5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4878F750-89DF-4AAA-BEC8-546D30795C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{136DF5E4-B4FF-4518-A1D3-9DD5166F4CEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="6" xr2:uid="{136DF5E4-B4FF-4518-A1D3-9DD5166F4CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="0401" sheetId="8" r:id="rId1"/>
@@ -1382,99 +1382,6 @@
     <t>Check the number of WPLABOR in MAXIMO</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Pick sampling data by executing the following SQL in maximodb:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>select top 5 * from CONTRACTLINE where STE_MIGRATIONID is not null and and linetype='ITEM';</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Take note the value of STE_MIGRATIONID
-Run the following SQL in coswindb:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SELECT ii.PK_ISS_ITEMS 
- , ii.ISS_ASK_QTY
- , di.PK_DEM_ISS 
- , di.DEM_WO_REF 
- , di.DEM_DEMANDER 
- , i.PK_ITEM_ 
- , i.ITEM_CD  
- , i.ITEM_SHORT  
- , i.STOCK_UNITS 
- , i.BUY_PRICE
- , si.S_ITEM_REF
- , lk.USER_ID AS DEMANDER_USER_ID
-FROM COSWIN.ISS_ITEMS ii 
-JOIN COSWIN.DEM_ISS di ON di.PK_DEM_ISS = ii.S_DEM_ISS_ITEM 
-LEFT JOIN COSWIN.ITEM_ i ON i.PK_ITEM_ = ii.S_ITEM_ISS 
-LEFT JOIN COSWIN.PORDER_ p ON P.PO_DEM_WO_REF = di.DEM_WO_REF 
-LEFT JOIN (
- -- can have multiple COSWIN.SUPL_ITEMS based on SUPPLIER name.
- -- since we do not know which supplier this item, just use the first row
- SELECT 
-  ii.PK_ISS_ITEMS, si.S_ITEM_REF 
-  , ROW_NUMBER() OVER (PARTITION BY ii.PK_ISS_ITEMS ORDER BY si.PK_SUPL_ITEMS) rn
- FROM COSWIN.ISS_ITEMS ii
- JOIN COSWIN.SUPL_ITEMS si ON si.S_ITEM_SUPL = ii.S_ITEM_ISS AND si.S_L_PO IS NULL 
-) si ON si.PK_ISS_ITEMS = ii.PK_ISS_ITEMS  AND rn=1
-LEFT JOIN (
- SELECT x.USR_NAME, wu.USER_ID, wu.USR_SIGNATURE
-  , ROW_NUMBER() OVER (PARTITION BY x.USR_NAME 
-   ORDER BY CASE WHEN trim(wu.USR_SIGNATURE) = TRIM(x.USR_NAME) THEN 0 ELSE 1 END, x.USR_NAME) RN 
- FROM (
-  SELECT DISTINCT x.DEM_DEMANDER AS USR_NAME FROM COSWIN.DEM_ISS x
- ) x
- LEFT JOIN coswin.WIN_USERS wu on UPPER(trim(wu.USR_SIGNATURE)) = UPPER(TRIM(x.USR_NAME)) 
-  OR UPPER(TRIM(wu.USER_ID)) = UPPER(TRIM(x.USR_NAME))
-  OR UPPER(TRIM(wu.USR_SIGNATURE)) LIKE concat(UPPER(TRIM(x.USR_NAME)),'%')
- WHERE x.USR_NAME IS NOT NULL 
-  --AND wu.USER_ID IS NULL 
- ORDER BY CASE WHEN wu.USER_ID IS NOT NULL THEN 0 ELSE 1 END, TRIM(x.USR_NAME) 
-  , CASE WHEN trim(wu.USR_SIGNATURE) = TRIM(x.USR_NAME) THEN 0 ELSE 1 END 
-  , TRIM(x.USR_NAME) 
-) lk ON lk.USR_NAME = di.DEM_DEMANDER AND lk.RN=1
-WHERE ii.PK_ISS_ITEMS IN (xxx);</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-(x is the previously noted STE_MIGRATIONID)</t>
-    </r>
-  </si>
-  <si>
     <t>MAX(WPITEMID) &lt;= maxreserved in MAXSEQUENCE</t>
   </si>
   <si>
@@ -2749,6 +2656,99 @@
   </si>
   <si>
     <t>Sample data comparison (PARENT Labtrans)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pick sampling data by executing the following SQL in maximodb:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select top 5 * from WPITEM where STE_MIGRATIONID is not null and and linetype='ITEM';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Take note the value of STE_MIGRATIONID
+Run the following SQL in coswindb:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT ii.PK_ISS_ITEMS 
+ , ii.ISS_ASK_QTY
+ , di.PK_DEM_ISS 
+ , di.DEM_WO_REF 
+ , di.DEM_DEMANDER 
+ , i.PK_ITEM_ 
+ , i.ITEM_CD  
+ , i.ITEM_SHORT  
+ , i.STOCK_UNITS 
+ , i.BUY_PRICE
+ , si.S_ITEM_REF
+ , lk.USER_ID AS DEMANDER_USER_ID
+FROM COSWIN.ISS_ITEMS ii 
+JOIN COSWIN.DEM_ISS di ON di.PK_DEM_ISS = ii.S_DEM_ISS_ITEM 
+LEFT JOIN COSWIN.ITEM_ i ON i.PK_ITEM_ = ii.S_ITEM_ISS 
+LEFT JOIN COSWIN.PORDER_ p ON P.PO_DEM_WO_REF = di.DEM_WO_REF 
+LEFT JOIN (
+ -- can have multiple COSWIN.SUPL_ITEMS based on SUPPLIER name.
+ -- since we do not know which supplier this item, just use the first row
+ SELECT 
+  ii.PK_ISS_ITEMS, si.S_ITEM_REF 
+  , ROW_NUMBER() OVER (PARTITION BY ii.PK_ISS_ITEMS ORDER BY si.PK_SUPL_ITEMS) rn
+ FROM COSWIN.ISS_ITEMS ii
+ JOIN COSWIN.SUPL_ITEMS si ON si.S_ITEM_SUPL = ii.S_ITEM_ISS AND si.S_L_PO IS NULL 
+) si ON si.PK_ISS_ITEMS = ii.PK_ISS_ITEMS  AND rn=1
+LEFT JOIN (
+ SELECT x.USR_NAME, wu.USER_ID, wu.USR_SIGNATURE
+  , ROW_NUMBER() OVER (PARTITION BY x.USR_NAME 
+   ORDER BY CASE WHEN trim(wu.USR_SIGNATURE) = TRIM(x.USR_NAME) THEN 0 ELSE 1 END, x.USR_NAME) RN 
+ FROM (
+  SELECT DISTINCT x.DEM_DEMANDER AS USR_NAME FROM COSWIN.DEM_ISS x
+ ) x
+ LEFT JOIN coswin.WIN_USERS wu on UPPER(trim(wu.USR_SIGNATURE)) = UPPER(TRIM(x.USR_NAME)) 
+  OR UPPER(TRIM(wu.USER_ID)) = UPPER(TRIM(x.USR_NAME))
+  OR UPPER(TRIM(wu.USR_SIGNATURE)) LIKE concat(UPPER(TRIM(x.USR_NAME)),'%')
+ WHERE x.USR_NAME IS NOT NULL 
+  --AND wu.USER_ID IS NULL 
+ ORDER BY CASE WHEN wu.USER_ID IS NOT NULL THEN 0 ELSE 1 END, TRIM(x.USR_NAME) 
+  , CASE WHEN trim(wu.USR_SIGNATURE) = TRIM(x.USR_NAME) THEN 0 ELSE 1 END 
+  , TRIM(x.USR_NAME) 
+) lk ON lk.USR_NAME = di.DEM_DEMANDER AND lk.RN=1
+WHERE ii.PK_ISS_ITEMS IN (xxx);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(x is the previously noted STE_MIGRATIONID)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3268,7 +3268,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -3298,7 +3298,7 @@
         <v>51</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
@@ -3328,7 +3328,7 @@
         <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>14</v>
@@ -3448,7 +3448,7 @@
         <v>56</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>49</v>
@@ -3475,13 +3475,13 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -3505,13 +3505,13 @@
         <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>66</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>46</v>
@@ -3736,7 +3736,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3749,7 +3749,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -3766,7 +3766,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3796,7 +3796,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3809,7 +3809,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>66</v>
@@ -3826,7 +3826,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3856,7 +3856,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3886,7 +3886,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3918,7 +3918,7 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
@@ -4020,7 +4020,7 @@
         <v>74</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -4050,7 +4050,7 @@
         <v>75</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
@@ -4080,7 +4080,7 @@
         <v>76</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>35</v>
@@ -4107,10 +4107,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>35</v>
@@ -4338,7 +4338,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4351,7 +4351,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -4368,7 +4368,7 @@
         <v>79</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4381,7 +4381,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>12</v>
@@ -4398,7 +4398,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4411,7 +4411,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>84</v>
@@ -4428,7 +4428,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4438,13 +4438,13 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -4459,7 +4459,7 @@
         <v>78</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4472,7 +4472,7 @@
         <v>95</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>84</v>
@@ -4490,7 +4490,7 @@
         <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4520,7 +4520,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4550,7 +4550,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4682,7 +4682,7 @@
         <v>87</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -4712,7 +4712,7 @@
         <v>88</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
@@ -4742,7 +4742,7 @@
         <v>89</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>14</v>
@@ -4772,7 +4772,7 @@
         <v>90</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
@@ -4922,7 +4922,7 @@
         <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>97</v>
@@ -5119,7 +5119,7 @@
         <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" ref="E3:E14" si="0">CONCATENATE(C3,"-",A3)</f>
@@ -5132,7 +5132,7 @@
         <v>102</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -5149,7 +5149,7 @@
         <v>79</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5162,7 +5162,7 @@
         <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>14</v>
@@ -5179,7 +5179,7 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5192,7 +5192,7 @@
         <v>104</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>14</v>
@@ -5209,7 +5209,7 @@
         <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" ref="E6" si="1">CONCATENATE(C6,"-",A6)</f>
@@ -5219,10 +5219,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
@@ -5239,7 +5239,7 @@
         <v>79</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5252,7 +5252,7 @@
         <v>106</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>35</v>
@@ -5269,7 +5269,7 @@
         <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5282,7 +5282,7 @@
         <v>105</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>35</v>
@@ -5299,7 +5299,7 @@
         <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5312,7 +5312,7 @@
         <v>107</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>12</v>
@@ -5329,7 +5329,7 @@
         <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" ref="E10" si="2">CONCATENATE(C10,"-",A10)</f>
@@ -5339,10 +5339,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>12</v>
@@ -5359,7 +5359,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5369,13 +5369,13 @@
         <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5389,7 +5389,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5402,7 +5402,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>8</v>
@@ -5419,7 +5419,7 @@
         <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5449,7 +5449,7 @@
         <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5480,10 +5480,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDD5F12-1F26-4860-A296-6FEE19BFBD64}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G4" sqref="G4"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5583,7 +5583,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -5643,7 +5643,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>110</v>
@@ -5750,7 +5750,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5763,7 +5763,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
@@ -5780,7 +5780,7 @@
         <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5793,7 +5793,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>12</v>
@@ -5810,7 +5810,7 @@
         <v>80</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5823,10 +5823,10 @@
         <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5840,7 +5840,7 @@
         <v>80</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5853,7 +5853,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>8</v>
@@ -5870,7 +5870,7 @@
         <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -5900,7 +5900,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6019,7 +6019,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6032,7 +6032,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>14</v>
@@ -6049,7 +6049,7 @@
         <v>81</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6062,7 +6062,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>12</v>
@@ -6079,7 +6079,7 @@
         <v>81</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6092,10 +6092,10 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6109,7 +6109,7 @@
         <v>81</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6122,7 +6122,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>8</v>
@@ -6139,7 +6139,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -6169,7 +6169,7 @@
         <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>